<commit_message>
changed random mapping logic, added santa emailid and child emailid to employees object, random mapping based on group
</commit_message>
<xml_diff>
--- a/SecretSantaNode/list.xlsx
+++ b/SecretSantaNode/list.xlsx
@@ -11,15 +11,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="13">
   <si>
     <t>mahikanthnag.yalamarthi@accoliteindia.com</t>
   </si>
   <si>
+    <t>Mahikanth Nag</t>
+  </si>
+  <si>
+    <t>Night</t>
+  </si>
+  <si>
+    <t>Idera</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Accolite</t>
+  </si>
+  <si>
     <t>babanag95@gmail.com</t>
   </si>
   <si>
+    <t>babanag</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
     <t>secretsanta.accolite@gmail.com</t>
+  </si>
+  <si>
+    <t>secretsanta</t>
+  </si>
+  <si>
+    <t>FedEx</t>
+  </si>
+  <si>
+    <t>Cambium</t>
   </si>
 </sst>
 </file>
@@ -96,116 +126,401 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
         <v>4.0</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
         <v>5.0</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
         <v>6.0</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
         <v>7.0</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
         <v>8.0</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
         <v>9.0</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
         <v>10.0</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
         <v>11.0</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
         <v>12.0</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
         <v>13.0</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
         <v>14.0</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
         <v>15.0</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
         <v>16.0</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
         <v>17.0</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
         <v>18.0</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
         <v>19.0</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1"/>

</xml_diff>